<commit_message>
mich tech northern michigan plots added, adjusted some formatting
</commit_message>
<xml_diff>
--- a/data/Game_Score/V2/Formula Graphic.xlsx
+++ b/data/Game_Score/V2/Formula Graphic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\Project\college_hockey\data\Game_Score\V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02C8FF0-885E-418F-B825-09E4033B441E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1A936E-A79B-424A-B11E-70EFC42964D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="-1020" windowWidth="25440" windowHeight="15990" xr2:uid="{66F3FCD2-025F-445A-A2FA-0D2FC6CBBAB0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{66F3FCD2-025F-445A-A2FA-0D2FC6CBBAB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <author>Justin</author>
   </authors>
   <commentList>
-    <comment ref="G2" authorId="0" shapeId="0" xr:uid="{D3301471-CEC3-4C39-8BC7-9D9DEFC25526}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{D3301471-CEC3-4C39-8BC7-9D9DEFC25526}">
       <text>
         <r>
           <rPr>
@@ -63,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{504C5033-8735-4B1F-9D7F-1D325A8EA04F}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{504C5033-8735-4B1F-9D7F-1D325A8EA04F}">
       <text>
         <r>
           <rPr>
@@ -87,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G15" authorId="0" shapeId="0" xr:uid="{A71CB205-99DD-4BB2-8BCA-755792F12C6F}">
+    <comment ref="G14" authorId="0" shapeId="0" xr:uid="{A71CB205-99DD-4BB2-8BCA-755792F12C6F}">
       <text>
         <r>
           <rPr>
@@ -270,12 +270,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Roboto Slab"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="1"/>
       <name val="Roboto Slab"/>
@@ -299,6 +293,13 @@
     </font>
     <font>
       <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="28"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -337,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -359,32 +360,38 @@
     <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -705,17 +712,17 @@
   </sheetPr>
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.5" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" customWidth="1"/>
-    <col min="3" max="3" width="2.85546875" style="14" customWidth="1"/>
-    <col min="4" max="4" width="27" style="15" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="13" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" style="11" customWidth="1"/>
+    <col min="4" max="4" width="27" style="12" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" style="10" customWidth="1"/>
     <col min="6" max="6" width="4.140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3" style="5" bestFit="1" customWidth="1"/>
@@ -724,286 +731,299 @@
     <col min="11" max="11" width="11" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="10"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A2" s="17"/>
-      <c r="G2" s="9" t="s">
+      <c r="B1" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="8">
+        <f>K2*1.75</f>
+        <v>0.97125000000000006</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8">
+        <f>K2*1.5</f>
+        <v>0.83250000000000002</v>
+      </c>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8">
+        <v>0.55500000000000005</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="29.25" x14ac:dyDescent="0.5">
       <c r="A3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>0</v>
+      <c r="B3" s="14"/>
+      <c r="E3" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G3" s="8">
         <f>K3*1.75</f>
-        <v>0.97125000000000006</v>
+        <v>0.79625000000000001</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8">
         <f>K3*1.5</f>
-        <v>0.83250000000000002</v>
+        <v>0.6825</v>
       </c>
       <c r="J3" s="8"/>
       <c r="K3" s="8">
-        <v>0.55500000000000005</v>
+        <v>0.45500000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="E4" s="13" t="s">
-        <v>21</v>
+      <c r="E4" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G4" s="8">
         <f>K4*1.75</f>
-        <v>0.79625000000000001</v>
+        <v>0.62124999999999997</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="8">
         <f>K4*1.5</f>
-        <v>0.6825</v>
+        <v>0.53249999999999997</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="8">
-        <v>0.45500000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="E5" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="3" t="s">
+        <v>0.35499999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="G6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="8">
-        <f>K5*1.75</f>
-        <v>0.62124999999999997</v>
-      </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8">
-        <f>K5*1.5</f>
-        <v>0.53249999999999997</v>
-      </c>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8">
-        <v>0.35499999999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="G7" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="9" t="s">
-        <v>24</v>
+      <c r="G7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="C8" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>9</v>
+      <c r="D8" s="13"/>
+      <c r="E8" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>12</v>
+      <c r="G8" s="8">
+        <v>0.08</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="D9" s="16"/>
-      <c r="E9" s="13" t="s">
-        <v>10</v>
+      <c r="D9" s="13"/>
+      <c r="E9" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G9" s="8">
-        <v>0.08</v>
+        <v>0.05</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="D10" s="16"/>
-      <c r="E10" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="D10" s="13"/>
+    </row>
+    <row r="11" spans="1:11" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="21"/>
+      <c r="D11" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="D11" s="16"/>
+      <c r="G11" s="8">
+        <v>7.4999999999999997E-2</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="C12" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>8</v>
+      <c r="D12" s="13"/>
+      <c r="E12" s="10" t="s">
+        <v>7</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G12" s="8">
-        <v>7.4999999999999997E-2</v>
+        <v>-7.4999999999999997E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="D13" s="16"/>
-      <c r="E13" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="D13" s="13"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:11" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="21"/>
+      <c r="D14" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="8">
-        <v>-7.4999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="D14" s="16"/>
-      <c r="G14" s="7"/>
+      <c r="G14" s="8">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="C15" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="4" t="s">
+      <c r="E15" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>17</v>
       </c>
       <c r="G15" s="8">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="E16" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="8">
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="G18" s="9" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="G17" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H18" s="9" t="s">
+      <c r="H17" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="I18" s="11" t="s">
+      <c r="I17" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
+      <c r="J17" s="17"/>
+      <c r="K17" s="17"/>
+    </row>
+    <row r="18" spans="1:11" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="21"/>
+      <c r="D18" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="8">
+        <v>1</v>
+      </c>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="C19" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>3</v>
+      <c r="E19" s="10" t="s">
+        <v>4</v>
       </c>
       <c r="G19" s="8">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="H19" s="8"/>
-      <c r="I19" s="12" t="s">
+      <c r="I19" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
+      <c r="J19" s="16"/>
+      <c r="K19" s="16"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="G20" s="8">
-        <v>2.5</v>
-      </c>
-      <c r="H20" s="8"/>
-      <c r="I20" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="9">
     <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="I18:K18"/>
     <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="I17:K17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="64" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
after first frint of draft_1
</commit_message>
<xml_diff>
--- a/data/Game_Score/V2/Formula Graphic.xlsx
+++ b/data/Game_Score/V2/Formula Graphic.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Desktop\Project\college_hockey\data\Game_Score\V2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1A936E-A79B-424A-B11E-70EFC42964D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D18517-77BC-48A2-80A5-67609F6E35A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{66F3FCD2-025F-445A-A2FA-0D2FC6CBBAB0}"/>
   </bookViews>
@@ -39,7 +39,7 @@
     <author>Justin</author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{D3301471-CEC3-4C39-8BC7-9D9DEFC25526}">
+    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{D3301471-CEC3-4C39-8BC7-9D9DEFC25526}">
       <text>
         <r>
           <rPr>
@@ -63,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{504C5033-8735-4B1F-9D7F-1D325A8EA04F}">
+    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{504C5033-8735-4B1F-9D7F-1D325A8EA04F}">
       <text>
         <r>
           <rPr>
@@ -87,7 +87,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G14" authorId="0" shapeId="0" xr:uid="{A71CB205-99DD-4BB2-8BCA-755792F12C6F}">
+    <comment ref="G17" authorId="0" shapeId="0" xr:uid="{A71CB205-99DD-4BB2-8BCA-755792F12C6F}">
       <text>
         <r>
           <rPr>
@@ -116,7 +116,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t>Goals</t>
   </si>
@@ -127,12 +127,6 @@
     <t>[PENALTIES]</t>
   </si>
   <si>
-    <t>Minor</t>
-  </si>
-  <si>
-    <t>Major</t>
-  </si>
-  <si>
     <t>Plus / Minus</t>
   </si>
   <si>
@@ -169,9 +163,6 @@
     <t>BASE</t>
   </si>
   <si>
-    <t>#</t>
-  </si>
-  <si>
     <t>+</t>
   </si>
   <si>
@@ -187,21 +178,6 @@
     <t>Assist 2</t>
   </si>
   <si>
-    <t>SHORT</t>
-  </si>
-  <si>
-    <t>CLOSE</t>
-  </si>
-  <si>
-    <t>5 ON 5</t>
-  </si>
-  <si>
-    <t>EVEN</t>
-  </si>
-  <si>
-    <t>A.G.S.</t>
-  </si>
-  <si>
     <t>[ SCORING ]</t>
   </si>
   <si>
@@ -211,23 +187,46 @@
     <t>[ FACEOFFS ]</t>
   </si>
   <si>
-    <t>[ TEAM ]</t>
-  </si>
-  <si>
     <t>[ Adjusted Game Score ]</t>
   </si>
   <si>
     <t>=</t>
   </si>
   <si>
-    <t>GitHub: JSmith1826</t>
+    <t>SHORTHANDED</t>
+  </si>
+  <si>
+    <t>CLOSE GAME</t>
+  </si>
+  <si>
+    <t>OTHER 5 on 5</t>
+  </si>
+  <si>
+    <t>Minor (2 min)</t>
+  </si>
+  <si>
+    <t>Major (5 min)</t>
+  </si>
+  <si>
+    <t>[ DEFENSE]</t>
+  </si>
+  <si>
+    <t>All data necessary to calculate AGS is available from CHN Box Scores and Advanced Metrics.</t>
+  </si>
+  <si>
+    <t>Adjusted Game Score or AGS is a custom metric, aggregating publicly available and standardized scoring, shot, faceoff, plus/minus, blocked shot, and penalty data into a unified value representing a player's single-game impact. 
+The metric was created by in 2023 by J.B. Smith and is a work in progress. The formula below is version 0.2</t>
+  </si>
+  <si>
+    <t>CLOSE GAME is defined by College Hockey News as within 1 goal (up 1, down 1, or tied) in the 1st and 2nd period 
+OR a tied even strength game in the 3rd period.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -241,11 +240,6 @@
       <name val="Roboto Slab"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Roboto Slab"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -287,23 +281,21 @@
       <name val="Roboto Slab"/>
     </font>
     <font>
-      <sz val="72"/>
-      <color theme="1"/>
-      <name val="Roboto Slab ExtraBold"/>
-    </font>
-    <font>
-      <sz val="22"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="28"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Roboto Slab"/>
+    </font>
+    <font>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Roboto Slab"/>
     </font>
   </fonts>
   <fills count="4">
@@ -321,7 +313,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -338,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -350,47 +342,69 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -710,323 +724,360 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K20"/>
+  <dimension ref="A2:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.5" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3" customWidth="1"/>
-    <col min="3" max="3" width="2.85546875" style="11" customWidth="1"/>
-    <col min="4" max="4" width="27" style="12" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" style="10" customWidth="1"/>
-    <col min="6" max="6" width="4.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="3" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="27" style="8" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" style="3" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="3.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="18" t="s">
+    <row r="2" spans="1:11" ht="189.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+    </row>
+    <row r="4" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="C4" s="13"/>
+      <c r="G4" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="19" t="s">
+    </row>
+    <row r="5" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="26"/>
+      <c r="G5" s="27">
+        <f>K5*1.75</f>
+        <v>0.97125000000000006</v>
+      </c>
+      <c r="H5" s="27"/>
+      <c r="I5" s="27">
+        <f>K5*1.5</f>
+        <v>0.83250000000000002</v>
+      </c>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27">
+        <v>0.55500000000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="26"/>
+      <c r="G6" s="27">
+        <f>K6*1.75</f>
+        <v>0.79625000000000001</v>
+      </c>
+      <c r="H6" s="27"/>
+      <c r="I6" s="27">
+        <f>K6*1.5</f>
+        <v>0.6825</v>
+      </c>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27">
+        <v>0.45500000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="D7" s="20"/>
+      <c r="E7" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="26"/>
+      <c r="G7" s="27">
+        <f>K7*1.75</f>
+        <v>0.62124999999999997</v>
+      </c>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27">
+        <f>K7*1.5</f>
+        <v>0.53249999999999997</v>
+      </c>
+      <c r="J7" s="27"/>
+      <c r="K7" s="27">
+        <v>0.35499999999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="G9" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="18"/>
+      <c r="G10" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="18"/>
+      <c r="G11" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="D12" s="22"/>
+      <c r="E12" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="18"/>
+      <c r="G12" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="D13" s="9"/>
+    </row>
+    <row r="14" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="26"/>
+      <c r="G14" s="27">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="F15" s="26"/>
+      <c r="G15" s="27">
+        <v>-7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="D16" s="9"/>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B17" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="28"/>
+      <c r="G17" s="27">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F18" s="26"/>
+      <c r="G18" s="27">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="G20" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+    </row>
+    <row r="21" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B21" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="26"/>
+      <c r="G21" s="27">
+        <v>1</v>
+      </c>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+    </row>
+    <row r="22" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="26"/>
+      <c r="G22" s="27">
+        <v>2.5</v>
+      </c>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:11" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="18"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="8">
-        <f>K2*1.75</f>
-        <v>0.97125000000000006</v>
-      </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8">
-        <f>K2*1.5</f>
-        <v>0.83250000000000002</v>
-      </c>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8">
-        <v>0.55500000000000005</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="29.25" x14ac:dyDescent="0.5">
-      <c r="A3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="14"/>
-      <c r="E3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" s="8">
-        <f>K3*1.75</f>
-        <v>0.79625000000000001</v>
-      </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8">
-        <f>K3*1.5</f>
-        <v>0.6825</v>
-      </c>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8">
-        <v>0.45500000000000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="E4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="8">
-        <f>K4*1.75</f>
-        <v>0.62124999999999997</v>
-      </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8">
-        <f>K4*1.5</f>
-        <v>0.53249999999999997</v>
-      </c>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8">
-        <v>0.35499999999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="G6" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H6" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="28.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="D8" s="13"/>
-      <c r="E8" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="8">
-        <v>0.08</v>
-      </c>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="D9" s="13"/>
-      <c r="E9" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="D10" s="13"/>
-    </row>
-    <row r="11" spans="1:11" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="21"/>
-      <c r="D11" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="8">
-        <v>7.4999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="D12" s="13"/>
-      <c r="E12" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="8">
-        <v>-7.4999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="D13" s="13"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:11" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="21"/>
-      <c r="D14" s="13" t="s">
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="24"/>
+      <c r="K24" s="24"/>
+    </row>
+    <row r="25" spans="1:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="8">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="E15" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="8">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="G17" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I17" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-    </row>
-    <row r="18" spans="1:11" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G18" s="8">
-        <v>1</v>
-      </c>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="E19" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="G19" s="8">
-        <v>2.5</v>
-      </c>
-      <c r="H19" s="8"/>
-      <c r="I19" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A20" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="24"/>
+      <c r="I25" s="24"/>
+      <c r="J25" s="24"/>
+      <c r="K25" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="I17:K17"/>
+  <mergeCells count="13">
+    <mergeCell ref="A25:K25"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A24:K24"/>
+    <mergeCell ref="B10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="B14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="B17:C18"/>
+    <mergeCell ref="B21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="B5:C6"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="64" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="6" scale="32" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>